<commit_message>
New Hasmap Test case
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8064F217-98F3-4A64-B8F5-D5BDC5DC5862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7404AD-421D-432B-BF8F-100988DFF27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -282,19 +282,19 @@
     <t>ABCDEF</t>
   </si>
   <si>
-    <t>newtest1@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest2@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest3@gmail.com</t>
-  </si>
-  <si>
     <t>testsa@test.com</t>
   </si>
   <si>
     <t>qwerty</t>
+  </si>
+  <si>
+    <t>newrr34r34rtest1@gmail.com</t>
+  </si>
+  <si>
+    <t>newte43534st2@gmail.com</t>
+  </si>
+  <si>
+    <t>new43535test3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1044,10 +1044,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>71</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>71</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>71</v>

</xml_diff>